<commit_message>
Created a ColumnBase class to have the static_choices property common between the 2 Column classes (header and value).
Details:

- Corrected doc string omissions from the exceptions.
- Moved the static_choices property method to ColumnBase.
- Moved the field, unique, default, required, static_choices, current_choices, and current_choices_converter arguments to the base class constructor.

This caused all of the static choices set by the model field to populate the header comments.

Files checked in: DataRepo/data/tests/submission_v3/multitracer_v3/study.xlsx DataRepo/loaders/base/table_column.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/submission_v3/multitracer_v3/study.xlsx
+++ b/DataRepo/data/tests/submission_v3/multitracer_v3/study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/submission_v3/multitracer_v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30027673-F379-0845-B199-39E1A06FA2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F8B8BB-089D-9E44-ACFE-5F89546F388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="4920" windowWidth="39940" windowHeight="21040" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7280" yWindow="4920" windowWidth="39940" windowHeight="21040" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="5" r:id="rId1"/>
@@ -27,8 +27,19 @@
     <sheet name="Peak Annotation Details" sheetId="12" r:id="rId12"/>
     <sheet name="Defaults" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -414,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
   <si>
     <t>Age</t>
   </si>
@@ -693,6 +704,9 @@
   </si>
   <si>
     <t>MS Run</t>
+  </si>
+  <si>
+    <t>Tracer</t>
   </si>
 </sst>
 </file>
@@ -10652,7 +10666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A071A6C0-1F50-2649-B578-4832509AE47D}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10672,7 +10688,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>38</v>
@@ -10733,7 +10749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295AAE7F-6F13-2E4E-BF80-D85D286842A4}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>